<commit_message>
making sure I pushed everything
</commit_message>
<xml_diff>
--- a/scripts/julia_scripts/results5_noStop.xlsx
+++ b/scripts/julia_scripts/results5_noStop.xlsx
@@ -5,44 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cookiemonster/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cookiemonster/Desktop/NOPE/intraday_nope_research/scripts/julia_scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DCAB45-3A6B-4446-9FC8-FCBAC5003ED2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01940079-39A9-224C-93B3-8C0AFDC65575}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="500" windowWidth="32400" windowHeight="20320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1200" yWindow="500" windowWidth="32400" windowHeight="20320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results5_noStop" sheetId="1" r:id="rId1"/>
     <sheet name="Means" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Means!$C$2:$C$16</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Means!$D$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Means!$C$2:$C$16</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Means!$D$1</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Means!$D$2:$D$16</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Means!$E$1</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Means!$E$2:$E$16</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Means!$C$2:$C$16</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Means!$D$1</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Means!$D$2:$D$16</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Means!$E$1</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Means!$E$2:$E$16</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Means!$D$2:$D$16</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Means!$C$2:$C$16</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Means!$D$1</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Means!$D$2:$D$16</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Means!$E$1</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Means!$E$2:$E$16</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Means!$E$1</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Means!$E$2:$E$16</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Means!$C$2:$C$16</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Means!$D$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Means!$D$2:$D$16</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Means!$E$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Means!$E$2:$E$16</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
@@ -3197,7 +3170,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> NOPE with "Window" on X-Axis</a:t>
+              <a:t> Short NOPE with "Window" on X-Axis</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -16019,16 +15992,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>31750</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16172,16 +16145,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>450850</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16208,16 +16181,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>336550</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16247,13 +16220,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>584200</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>273050</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>44450</xdr:rowOff>
     </xdr:to>
@@ -16609,8 +16582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K277"/>
   <sheetViews>
-    <sheetView topLeftCell="O72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA92" sqref="AA92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26611,8 +26584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C84E6C0-687E-BB4A-AF9C-323D6FF416CD}">
   <dimension ref="C1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="R33" sqref="R33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>